<commit_message>
Translate Bill of Material
</commit_message>
<xml_diff>
--- a/Bill_of_Material.xlsx
+++ b/Bill_of_Material.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Documents/GitHub/FreeVarioGauge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Libelle/OpenVario/e-Vario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF537F86-3E03-CD4F-B5EE-53CE915ED769}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C3B11C-300E-A547-8957-7C364D89672F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A71850B3-3A10-CA42-999C-A02A84AA5A96}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="158">
   <si>
     <t>Value</t>
   </si>
@@ -60,18 +60,12 @@
     <t>https://www.ebay.de/itm/Espressif-ESP32-WLAN-Dev-Kit-Board-Development-Bluetooth-Wifi-v1-Deutsche-Post/163771189294?ssPageName=STRK%3AMEBIDX%3AIT&amp;_trksid=p2057872.m2749.l2649</t>
   </si>
   <si>
-    <t>Präz.-Buchsenleisten 2,54 mm, 1X15</t>
-  </si>
-  <si>
     <t>Reichelt</t>
   </si>
   <si>
     <t>MPE 115-1-015</t>
   </si>
   <si>
-    <t>Buchsenleiste, 8-pol</t>
-  </si>
-  <si>
     <t>SV2</t>
   </si>
   <si>
@@ -96,21 +90,12 @@
     <t>X2</t>
   </si>
   <si>
-    <t>SMD-Vielschicht-Keramikkondensator 10N</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
     <t>X7R-G0805 10N</t>
   </si>
   <si>
-    <t>SMD-Vielschicht-Keramikkondensator 100N</t>
-  </si>
-  <si>
-    <t>SMD-Vielschichtkondensator G0805 - 10µF 16V</t>
-  </si>
-  <si>
     <t>X5R-G0805 10/16</t>
   </si>
   <si>
@@ -129,99 +114,54 @@
     <t>SMD-0805 10,0K</t>
   </si>
   <si>
-    <t>Stiftleisten 2,54 mm, 2X05, gewinkelt</t>
-  </si>
-  <si>
     <t>MPE 088-2-010</t>
   </si>
   <si>
     <t>X3</t>
   </si>
   <si>
-    <t>36pol. Stiftleiste, gewinkelt</t>
-  </si>
-  <si>
     <t>Speaker</t>
   </si>
   <si>
     <t>SL 1X36W 2,54</t>
   </si>
   <si>
-    <t>Micro Lautsprecher Speaker 35 mm 4 Ohm 3W</t>
-  </si>
-  <si>
     <t>https://www.ebay.de/itm/Rund-Micro-Lautsprecher-Speaker-35-mm-4-Ohm-3W-fur-DIY-Reparatur/332662823028</t>
   </si>
   <si>
     <t>Vario Encoder Board</t>
   </si>
   <si>
-    <t>Drehpotentiometer, 25 kOhm</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
     <t>PIH T16SHM4N253B</t>
   </si>
   <si>
-    <t>Buchsenleiste, 10-pol</t>
-  </si>
-  <si>
     <t>RND 205-00654</t>
   </si>
   <si>
-    <t>Kippschalter 6A-125VAC, 1x Ein-Aus-Ein</t>
-  </si>
-  <si>
     <t>MS 500C</t>
   </si>
   <si>
-    <t>Drehencoder</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>https://www.ebay.de/itm/Bourns-Mechanical-Encoder-Rotary-Incremental-Tastend-5V-2Channel-2-Stück/361917632981?ssPageName=STRK%3AMEBIDX%3AIT&amp;_trksid=p2057872.m2749.l2649</t>
-  </si>
-  <si>
-    <t>Hohlschrauben (wie z.B. beim Funke ATR833)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUNDKNOPF 10, ohne Strich, 3mm Achsbohrung </t>
-  </si>
-  <si>
     <t>https://www.okw.com/</t>
   </si>
   <si>
-    <t>A2510030</t>
-  </si>
-  <si>
-    <t>Deckel 10, ohne Strich</t>
-  </si>
-  <si>
     <t>A4110000</t>
   </si>
   <si>
     <t>Q1, Q2</t>
   </si>
   <si>
-    <t>JST - Crimpkontakt, Buchse - XH</t>
-  </si>
-  <si>
     <t>JST XH CKB</t>
   </si>
   <si>
-    <t>JST - Stiftleiste, gerade, 1x3-polig - XH</t>
-  </si>
-  <si>
     <t>JST XH3P ST</t>
   </si>
   <si>
-    <t>JST - Buchsengehäuse, 1x3-polig - XH</t>
-  </si>
-  <si>
     <t>JST XH3P BU</t>
   </si>
   <si>
@@ -231,12 +171,6 @@
     <t>NCP 1117 ST33T3G </t>
   </si>
   <si>
-    <t>JST - Buchsengehäuse, 1x2-polig - XH</t>
-  </si>
-  <si>
-    <t>JST - Stiftleiste, 90°, 1x2-polig - XH</t>
-  </si>
-  <si>
     <t>JST XH2P ST90</t>
   </si>
   <si>
@@ -246,9 +180,6 @@
     <t>﻿STF-WOELBKLAPPEN</t>
   </si>
   <si>
-    <t>Schiebeschalter 1x UM, stehend</t>
-  </si>
-  <si>
     <t>X4</t>
   </si>
   <si>
@@ -261,18 +192,12 @@
     <t>X7R-G0805 100N</t>
   </si>
   <si>
-    <t>Kühlkörper SMD 6,3 x4,8x 5,0mm</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
     <t>ICK SMD A5</t>
   </si>
   <si>
-    <t>Wärmeleitfolie selbstklebend</t>
-  </si>
-  <si>
     <t>https://www.ebay.de/itm/EC360-ADHESIVE-WHITE-Wärmeleitfolie-kleber-50x50mm-Doppelseitig-3W-mK-WLPad/113931974912?ssPageName=STRK%3AMEBIDX%3AIT&amp;_trksid=p2057872.m2749.l2649</t>
   </si>
   <si>
@@ -280,9 +205,6 @@
   </si>
   <si>
     <t>C1</t>
-  </si>
-  <si>
-    <t>SMD-Vielschichtkondensator G0805 - 1,0µF 50V</t>
   </si>
   <si>
     <t>X7R-G0805 1,0/50</t>
@@ -359,6 +281,150 @@
     <t>EA WF050-40ST</t>
   </si>
   <si>
+    <t>MOLEX 541044031</t>
+  </si>
+  <si>
+    <t>C164172</t>
+  </si>
+  <si>
+    <t>ZIF SMD</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C83170</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>C49678</t>
+  </si>
+  <si>
+    <t>1µF</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>C77083</t>
+  </si>
+  <si>
+    <t>C77075</t>
+  </si>
+  <si>
+    <t>PAM8302A</t>
+  </si>
+  <si>
+    <t>C113367</t>
+  </si>
+  <si>
+    <t>MSOP8</t>
+  </si>
+  <si>
+    <t>PAM8302AASCR</t>
+  </si>
+  <si>
+    <t>C26537</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>C17314</t>
+  </si>
+  <si>
+    <t>C84376</t>
+  </si>
+  <si>
+    <t>https://www.luna-electronic.de/de/tft-displays/newhaven-display-nhd-2-4-240320cf-csxn-f-2-4-sunlight-readable-tft.html</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>MPE 115-1-007</t>
+  </si>
+  <si>
+    <t>Ebay, Mouser</t>
+  </si>
+  <si>
+    <t>215877-1</t>
+  </si>
+  <si>
+    <t>C15, C16</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>NPO-G0805 220P</t>
+  </si>
+  <si>
+    <t>EMI Suppression Filter SMD0603 BLM18 120 Ohm</t>
+  </si>
+  <si>
+    <t>BLM18AG 121</t>
+  </si>
+  <si>
+    <t>C9, C11, C14, C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>RND 0805 1 68K</t>
+  </si>
+  <si>
+    <t>RND 0805 1 33K</t>
+  </si>
+  <si>
+    <t>RND 0805 1 820</t>
+  </si>
+  <si>
+    <t>RND 0805 1 470</t>
+  </si>
+  <si>
+    <t>RND 0805 1 330</t>
+  </si>
+  <si>
+    <t>KEM X5R0805 4,7U</t>
+  </si>
+  <si>
+    <t>BC 848C SMD</t>
+  </si>
+  <si>
+    <t>Precision sockets 2,54 mm, 1X15</t>
+  </si>
+  <si>
     <r>
       <t>EA WF050-</t>
     </r>
@@ -376,182 +442,119 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri Light (Überschriften)"/>
       </rPr>
-      <t>ZIFF-Stecker</t>
+      <t>ZIFF conector</t>
     </r>
   </si>
   <si>
-    <t>MOLEX 541044031</t>
-  </si>
-  <si>
-    <t>C164172</t>
-  </si>
-  <si>
-    <t>ZIF SMD</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C83170</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>C49678</t>
-  </si>
-  <si>
-    <t>1µF</t>
-  </si>
-  <si>
-    <t>10µF</t>
-  </si>
-  <si>
-    <t>C77083</t>
-  </si>
-  <si>
-    <t>C77075</t>
-  </si>
-  <si>
-    <t>PAM8302A</t>
-  </si>
-  <si>
-    <t>C113367</t>
-  </si>
-  <si>
-    <t>MSOP8</t>
-  </si>
-  <si>
-    <t>PAM8302AASCR</t>
-  </si>
-  <si>
-    <t>C26537</t>
-  </si>
-  <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>C17314</t>
-  </si>
-  <si>
-    <t>C84376</t>
-  </si>
-  <si>
-    <t>https://www.luna-electronic.de/de/tft-displays/newhaven-display-nhd-2-4-240320cf-csxn-f-2-4-sunlight-readable-tft.html</t>
-  </si>
-  <si>
-    <t>Stapelleiste 2x4 h=26,5mm</t>
-  </si>
-  <si>
-    <t>Stapelleiste 2x2 h=26,5mm</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>Präz.-Buchsenleisten 2,54 mm, 1x7</t>
-  </si>
-  <si>
-    <t>MPE 115-1-007</t>
-  </si>
-  <si>
-    <t>Ebay, Mouser</t>
-  </si>
-  <si>
-    <t>215877-1</t>
-  </si>
-  <si>
-    <t>C15, C16</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>SMD-Vielschicht-Keramikkondensator 220P, 5%</t>
-  </si>
-  <si>
-    <t>NPO-G0805 220P</t>
-  </si>
-  <si>
-    <t>EMI Suppression Filter SMD0603 BLM18 120 Ohm</t>
-  </si>
-  <si>
-    <t>BLM18AG 121</t>
-  </si>
-  <si>
-    <t>C9, C11, C14, C17</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>SMD-Widerstand, 0805, 68 kOhm</t>
-  </si>
-  <si>
-    <t>RND 0805 1 68K</t>
-  </si>
-  <si>
-    <t>SMD-Widerstand, 0805, 33 kOhm</t>
-  </si>
-  <si>
-    <t>RND 0805 1 33K</t>
-  </si>
-  <si>
-    <t>SMD-Widerstand, 0805, 820 Ohm</t>
-  </si>
-  <si>
-    <t>RND 0805 1 820</t>
-  </si>
-  <si>
-    <t>SMD-Widerstand, 0805, 470 Ohm</t>
-  </si>
-  <si>
-    <t>RND 0805 1 470</t>
-  </si>
-  <si>
-    <t>SMD-Widerstand, 0805, 330 Ohm</t>
-  </si>
-  <si>
-    <t>RND 0805 1 330</t>
-  </si>
-  <si>
-    <t>Vielschicht-Kerko, 4,7µF, 25V</t>
-  </si>
-  <si>
-    <t>KEM X5R0805 4,7U</t>
-  </si>
-  <si>
-    <t>Bipolartransistor, NPN</t>
-  </si>
-  <si>
-    <t>BC 848C SMD</t>
+    <t>SMD chip resistor, 0805, 10 kOhm</t>
+  </si>
+  <si>
+    <t>SMD chip resistor, 0805, 68 kOhm</t>
+  </si>
+  <si>
+    <t>SMD chip resistor, 0805, 33 kOhm</t>
+  </si>
+  <si>
+    <t>SMD chip resistor, 0805, 820 Ohm</t>
+  </si>
+  <si>
+    <t>SMD chip resistor, 0805, 470 Ohm</t>
+  </si>
+  <si>
+    <t>SMD chip resistor, 0805, 330 Ohm</t>
+  </si>
+  <si>
+    <t>SMD multilayer capacitor G0805 - 1,0µF 50V</t>
+  </si>
+  <si>
+    <t>SMD multilayer capacitor G0805 - 10µF 16V</t>
+  </si>
+  <si>
+    <t>SMD multilayer ceramic capacitor 10N</t>
+  </si>
+  <si>
+    <t>SMD multilayer ceramic capacitor 100N</t>
+  </si>
+  <si>
+    <t>SMD multilayer ceramic capacitor 220P, 5%</t>
+  </si>
+  <si>
+    <t>multilayer ceramic capacitor, 4,7µF, 25V</t>
+  </si>
+  <si>
+    <t>transistor, NPN</t>
+  </si>
+  <si>
+    <t>Heat sink SMD 6,3 x4,8x 5,0mm</t>
+  </si>
+  <si>
+    <t>Pin headers 2.54 mm, 2X05, angled</t>
+  </si>
+  <si>
+    <t>Stack bar 2x4 h=26,5mm</t>
+  </si>
+  <si>
+    <t>Stack bar 2x2 h=26,5mm</t>
+  </si>
+  <si>
+    <t>Slide switch 1x UM, upright</t>
+  </si>
+  <si>
+    <t>Precision sockets 2,54 mm, 1x7</t>
+  </si>
+  <si>
+    <t>2-pin header, angled</t>
+  </si>
+  <si>
+    <t>Micro Speaker 35 mm 4 Ohm 3W</t>
+  </si>
+  <si>
+    <t>JST - crimp contact, socket - XH</t>
+  </si>
+  <si>
+    <t>Potentiometer, 25 kOhm</t>
+  </si>
+  <si>
+    <t>Pinheader female, 10-pin</t>
+  </si>
+  <si>
+    <t>Pinheader female, 8-pin</t>
+  </si>
+  <si>
+    <t>JST - pin header, straight, 1x3-pin - XH</t>
+  </si>
+  <si>
+    <t>JST - socket housing, 1x3-pin - XH</t>
+  </si>
+  <si>
+    <t>JST — pin header, 90°, 1x2-pin - XH</t>
+  </si>
+  <si>
+    <t>JST — socket housing, 1x2-pin - XH</t>
+  </si>
+  <si>
+    <t>Toggle switch 6A-125VAC, 1x On-Off-ON</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Banjo bolts (wie z.B. beim Funke ATR833)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROUND KNOB 10, WITHOUT LINE, 4mm Bore hole </t>
+  </si>
+  <si>
+    <t>A2510040</t>
+  </si>
+  <si>
+    <t>COVER 10, WITHOUT LINE</t>
+  </si>
+  <si>
+    <t>Alps STEC11B03</t>
+  </si>
+  <si>
+    <t>Self-adhesive thermal foil</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1371,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1390,260 +1393,260 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3">
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="C19" s="3">
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1651,75 +1654,75 @@
         <v>131</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1">
       <c r="A25" s="3" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -1730,79 +1733,79 @@
     </row>
     <row r="26" spans="1:6" s="4" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="3" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="3" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1821,62 +1824,62 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1886,10 +1889,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="9" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C38" s="9">
         <v>1</v>
@@ -1900,41 +1903,41 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1943,94 +1946,94 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
         <v>11</v>
-      </c>
-      <c r="E41" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2038,127 +2041,126 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="D56" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2167,35 +2169,35 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2271,156 +2273,156 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2468,44 +2470,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2588,44 +2590,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>

<commit_message>
Updates because of mute with PTT
</commit_message>
<xml_diff>
--- a/Bill_of_Material.xlsx
+++ b/Bill_of_Material.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Libelle/OpenVario/e-Vario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Libelle/OpenVario/e-Vario/Instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FBA9F5-E750-3F49-8A08-2DE269E6D56B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9E11AE-5B96-6347-935F-DF51BA844D54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A71850B3-3A10-CA42-999C-A02A84AA5A96}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="162">
   <si>
     <t>Value</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>NCP 1117 ST33T3G </t>
-  </si>
-  <si>
-    <t>JST XH2P BU</t>
   </si>
   <si>
     <t>﻿STF-WOELBKLAPPEN</t>
@@ -510,9 +507,6 @@
   </si>
   <si>
     <t>JST - socket housing, 1x3-pin - XH</t>
-  </si>
-  <si>
-    <t>JST — socket housing, 1x2-pin - XH</t>
   </si>
   <si>
     <t>Toggle switch 6A-125VAC, 1x On-Off-ON</t>
@@ -1035,7 +1029,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1392,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1411,7 +1405,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1425,7 +1419,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1442,10 +1436,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1454,7 +1448,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1468,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
         <v>94</v>
-      </c>
-      <c r="E9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1493,7 +1487,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1505,15 +1499,15 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
@@ -1522,16 +1516,16 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1540,16 +1534,16 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1558,16 +1552,16 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1576,16 +1570,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1594,16 +1588,16 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1612,13 +1606,13 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -1635,10 +1629,10 @@
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3">
         <v>5</v>
@@ -1647,15 +1641,15 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3">
         <v>4</v>
@@ -1664,15 +1658,15 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -1686,10 +1680,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="3">
         <v>2</v>
@@ -1698,15 +1692,15 @@
         <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1715,15 +1709,15 @@
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -1732,15 +1726,15 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="3">
         <v>2</v>
@@ -1749,12 +1743,12 @@
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="4" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>23</v>
@@ -1768,10 +1762,10 @@
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -1780,7 +1774,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -1789,7 +1783,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1803,7 +1797,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>39</v>
@@ -1815,12 +1809,12 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
@@ -1829,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -1859,10 +1853,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1876,10 +1870,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -1888,16 +1882,16 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1911,7 +1905,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
@@ -1924,10 +1918,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" s="9">
         <v>1</v>
@@ -1938,41 +1932,41 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
         <v>47</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
         <v>92</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -1989,7 +1983,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
@@ -2006,7 +2000,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -2018,15 +2012,15 @@
         <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>143</v>
+      <c r="A45" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2035,15 +2029,15 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2052,15 +2046,15 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2074,7 +2068,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B48" t="s">
         <v>15</v>
@@ -2083,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -2103,7 +2097,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -2115,12 +2109,12 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
@@ -2137,7 +2131,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>19</v>
@@ -2154,7 +2148,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
@@ -2171,7 +2165,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
@@ -2188,7 +2182,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2202,7 +2196,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
         <v>36</v>
@@ -2211,12 +2205,12 @@
         <v>1</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -2225,7 +2219,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2234,12 +2228,12 @@
         <v>37</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2328,16 +2322,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2348,24 +2342,24 @@
         <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2373,97 +2367,97 @@
         <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2471,13 +2465,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2525,16 +2519,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2542,27 +2536,27 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2645,16 +2639,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2662,27 +2656,27 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>

<commit_message>
Remote Stick can control FreeVario
</commit_message>
<xml_diff>
--- a/Bill_of_Material.xlsx
+++ b/Bill_of_Material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Documents/GitHub/FreeVarioGauge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A679E-0FB7-A04D-BA0F-F890D8568DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C2508C-B993-0E44-B0EE-45659224C903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A71850B3-3A10-CA42-999C-A02A84AA5A96}"/>
   </bookViews>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE93BCC-B60F-D148-9D08-040AD6C1FD16}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updates for tag 1.1.4
</commit_message>
<xml_diff>
--- a/Bill_of_Material.xlsx
+++ b/Bill_of_Material.xlsx
@@ -8,15 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Documents/GitHub/FreeVarioGauge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C2508C-B993-0E44-B0EE-45659224C903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443D1D04-7EFD-DA41-B8A0-F71BC5B917C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A71850B3-3A10-CA42-999C-A02A84AA5A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Vario" sheetId="1" r:id="rId1"/>
-    <sheet name="BOM-PCB1" sheetId="2" r:id="rId2"/>
-    <sheet name="BOM-PCB2" sheetId="3" r:id="rId3"/>
-    <sheet name="BOM-PCB3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>Value</t>
   </si>
@@ -108,9 +105,6 @@
     <t>Vario Board 2</t>
   </si>
   <si>
-    <t>SMD-Widerstand, 0805, 10 kOhm</t>
-  </si>
-  <si>
     <t>SMD-0805 10,0K</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>JST XH3P BU</t>
   </si>
   <si>
-    <t>NCP 1117 ST33T3G </t>
-  </si>
-  <si>
     <t>﻿STF-WOELBKLAPPEN</t>
   </si>
   <si>
@@ -168,15 +159,9 @@
     <t>SS ESP101</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4</t>
-  </si>
-  <si>
     <t>X7R-G0805 100N</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C5, C8</t>
   </si>
   <si>
@@ -186,135 +171,13 @@
     <t>X7R-G0805 1,0/50</t>
   </si>
   <si>
-    <t>C9, C11, C14</t>
-  </si>
-  <si>
-    <t>C6, C7, C10, C12, C13</t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>NCP 1117 ST50T3G</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>LCSC Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>optional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <t>SO-16</t>
-  </si>
-  <si>
-    <t>C143432</t>
-  </si>
-  <si>
     <t>EA WF050-40ST</t>
   </si>
   <si>
-    <t>MOLEX 541044031</t>
-  </si>
-  <si>
-    <t>C164172</t>
-  </si>
-  <si>
-    <t>ZIF SMD</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C83170</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>C49678</t>
-  </si>
-  <si>
-    <t>1µF</t>
-  </si>
-  <si>
-    <t>10µF</t>
-  </si>
-  <si>
-    <t>C77083</t>
-  </si>
-  <si>
-    <t>C77075</t>
-  </si>
-  <si>
     <t>PAM8302A</t>
-  </si>
-  <si>
-    <t>C113367</t>
-  </si>
-  <si>
-    <t>MSOP8</t>
-  </si>
-  <si>
-    <t>PAM8302AASCR</t>
-  </si>
-  <si>
-    <t>C26537</t>
-  </si>
-  <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>C17314</t>
-  </si>
-  <si>
-    <t>C84376</t>
   </si>
   <si>
     <t>https://www.luna-electronic.de/de/tft-displays/newhaven-display-nhd-2-4-240320cf-csxn-f-2-4-sunlight-readable-tft.html</t>
@@ -579,7 +442,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,25 +478,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light (Überschriften)"/>
@@ -659,21 +503,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -681,42 +519,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1038,7 +854,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -1362,7 +1178,7 @@
     <col min="16133" max="16133" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1379,12 +1195,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1392,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1409,9 +1225,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1423,9 +1239,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1440,12 +1256,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1454,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1468,14 +1284,14 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
@@ -1491,9 +1307,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1505,15 +1321,15 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
@@ -1522,16 +1338,16 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1540,16 +1356,16 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1558,16 +1374,16 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1576,16 +1392,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1594,16 +1410,16 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1612,13 +1428,13 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -1633,12 +1449,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19" s="3">
         <v>5</v>
@@ -1647,15 +1463,15 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C20" s="3">
         <v>4</v>
@@ -1664,15 +1480,15 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1684,12 +1500,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3">
         <v>2</v>
@@ -1698,15 +1514,15 @@
         <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1715,15 +1531,15 @@
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -1732,15 +1548,15 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C25" s="3">
         <v>2</v>
@@ -1749,12 +1565,12 @@
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>23</v>
@@ -1766,33 +1582,33 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1">
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1806,12 +1622,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -1820,67 +1636,67 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" t="s">
-        <v>157</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" t="s">
-        <v>29</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1888,26 +1704,26 @@
       <c r="D36" s="2"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="9">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="6">
         <v>1</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="E37" s="7"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1916,15 +1732,15 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1933,12 +1749,12 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -1953,29 +1769,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
         <v>30</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1984,15 +1800,15 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2001,16 +1817,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" t="s">
-        <v>43</v>
-      </c>
       <c r="C44">
         <v>1</v>
       </c>
@@ -2018,15 +1834,15 @@
         <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -2035,12 +1851,12 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
         <v>15</v>
@@ -2049,31 +1865,31 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B50" t="s">
-        <v>33</v>
-      </c>
       <c r="C50">
         <v>1</v>
       </c>
@@ -2081,12 +1897,12 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
@@ -2098,12 +1914,12 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>19</v>
@@ -2115,12 +1931,12 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
@@ -2132,12 +1948,12 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
@@ -2149,12 +1965,12 @@
         <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2163,61 +1979,61 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" t="s">
-        <v>36</v>
-      </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
@@ -2226,43 +2042,43 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
     </row>
   </sheetData>
@@ -2274,441 +2090,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE57722-5B75-1D40-B9DC-B066A479B666}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="C15" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://lcsc.com/product-detail/RS232-ICs_Maxim-Integrated_MAX3232ECWE_Maxim-Integrated-MAX3232ECWE_C143432.html" xr:uid="{FFB8C294-ADB0-F040-8E94-CA7FA2EA3011}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://lcsc.com/product-detail/FFC-FPC-Connectors_MOLEX_541044031_MOLEX-541044031_C164172.html" xr:uid="{A7338377-6668-2044-8707-7702B89446DA}"/>
-    <hyperlink ref="D5" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_10nF-103-10-50V_C83170.html" xr:uid="{898EF980-0C37-1645-A0A7-204CDB314404}"/>
-    <hyperlink ref="D7" r:id="rId4" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_muRata_GRM21BR71H105KA12L_1uF-105-10-50V_C77083.html" xr:uid="{1D7CFD7E-0378-D34D-93C2-E2A1F7CCE8B6}"/>
-    <hyperlink ref="D9" r:id="rId5" display="https://lcsc.com/product-detail/Audio-Power-OpAmps_Diodes-Incorporated_PAM8302AASCR_Diodes-Incorporated-PAM8302AASCR_C113367.html" xr:uid="{E725EF93-6260-8C48-A42F-BB8CA19F9EFB}"/>
-    <hyperlink ref="A9" r:id="rId6" display="https://lcsc.com/product-detail/Audio-Power-OpAmps_Diodes-Incorporated_PAM8302AASCR_Diodes-Incorporated-PAM8302AASCR_C113367.html" xr:uid="{D6D8886E-D7E2-A846-BA93-6765604167F3}"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_ON-Semiconductor-ON-NCP1117ST50T3G_C17314.html" xr:uid="{1C2BF8A9-1D03-DD4D-87A2-7145C42F989B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B9D977-3A0D-9F42-A6D8-BF8241070D0D}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="3"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="3"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="3"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="3"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="3"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="3"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5151FA7D-8764-CA4A-9E1E-220B2BFCB1B2}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="3"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="3"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="3"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="3"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="3"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="3"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>